<commit_message>
First version pushed to GitHub
</commit_message>
<xml_diff>
--- a/langame.xlsx
+++ b/langame.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="20" windowWidth="25600" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="360" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="WORDLDS" sheetId="1" r:id="rId1"/>
@@ -19,28 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="160">
-  <si>
-    <t>SPANISH</t>
-  </si>
-  <si>
-    <t>PORTUGUESE</t>
-  </si>
-  <si>
-    <t>CATALAN</t>
-  </si>
-  <si>
-    <t>FRENCH</t>
-  </si>
-  <si>
-    <t>ITALIAN</t>
-  </si>
-  <si>
-    <t>RUSSIAN</t>
-  </si>
-  <si>
-    <t>ENGLISH</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="237">
   <si>
     <t>Hombre</t>
   </si>
@@ -168,9 +147,6 @@
     <t>Маленький малчик</t>
   </si>
   <si>
-    <t>Маленькая дебочка</t>
-  </si>
-  <si>
     <t>Ребенок</t>
   </si>
   <si>
@@ -499,6 +475,261 @@
   </si>
   <si>
     <t>Dinner</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>Arriba</t>
+  </si>
+  <si>
+    <t>Abajo</t>
+  </si>
+  <si>
+    <t>Derecha</t>
+  </si>
+  <si>
+    <t>Izquierda</t>
+  </si>
+  <si>
+    <t>Atrás</t>
+  </si>
+  <si>
+    <t>Aquí</t>
+  </si>
+  <si>
+    <t>Allí</t>
+  </si>
+  <si>
+    <t>Qui</t>
+  </si>
+  <si>
+    <t>Enllà</t>
+  </si>
+  <si>
+    <t>Esto</t>
+  </si>
+  <si>
+    <t>Ici</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>There</t>
+  </si>
+  <si>
+    <t>Здесь, Вот</t>
+  </si>
+  <si>
+    <t>Там</t>
+  </si>
+  <si>
+    <t>Là</t>
+  </si>
+  <si>
+    <t>Lá</t>
+  </si>
+  <si>
+    <t>Isto</t>
+  </si>
+  <si>
+    <t>This</t>
+  </si>
+  <si>
+    <t>That</t>
+  </si>
+  <si>
+    <t>Eso, Aquello</t>
+  </si>
+  <si>
+    <t>Isso, Aquilo</t>
+  </si>
+  <si>
+    <t>Ce ici</t>
+  </si>
+  <si>
+    <t>Ce là</t>
+  </si>
+  <si>
+    <t>Això</t>
+  </si>
+  <si>
+    <t>Allò</t>
+  </si>
+  <si>
+    <t>Questo</t>
+  </si>
+  <si>
+    <t>Quelo</t>
+  </si>
+  <si>
+    <t>Это</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Delante</t>
+  </si>
+  <si>
+    <t>Detrás</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>Giù</t>
+  </si>
+  <si>
+    <t>Sinistra</t>
+  </si>
+  <si>
+    <t>Destra</t>
+  </si>
+  <si>
+    <t>Esquerra</t>
+  </si>
+  <si>
+    <t>Dreta</t>
+  </si>
+  <si>
+    <t>Adalt</t>
+  </si>
+  <si>
+    <t>Abaix</t>
+  </si>
+  <si>
+    <t>Endavant</t>
+  </si>
+  <si>
+    <t>Darrera</t>
+  </si>
+  <si>
+    <t>Dietro</t>
+  </si>
+  <si>
+    <t>Avanti</t>
+  </si>
+  <si>
+    <t>Dessus</t>
+  </si>
+  <si>
+    <t>Dessous</t>
+  </si>
+  <si>
+    <t>Droite</t>
+  </si>
+  <si>
+    <t>Gauche</t>
+  </si>
+  <si>
+    <t>Avant</t>
+  </si>
+  <si>
+    <t>Derrière</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Non</t>
+  </si>
+  <si>
+    <t>Oui</t>
+  </si>
+  <si>
+    <t>Нет</t>
+  </si>
+  <si>
+    <t>Да</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Not</t>
+  </si>
+  <si>
+    <t>За</t>
+  </si>
+  <si>
+    <t>Слева</t>
+  </si>
+  <si>
+    <t>Вниз</t>
+  </si>
+  <si>
+    <t>Вверх</t>
+  </si>
+  <si>
+    <t>Abaixo</t>
+  </si>
+  <si>
+    <t>Acima</t>
+  </si>
+  <si>
+    <t>Frente</t>
+  </si>
+  <si>
+    <t>Esquerda</t>
+  </si>
+  <si>
+    <t>Direita</t>
+  </si>
+  <si>
+    <t>Перед</t>
+  </si>
+  <si>
+    <t>Справа</t>
+  </si>
+  <si>
+    <t>Маленькая девочка</t>
   </si>
 </sst>
 </file>
@@ -998,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1017,569 +1248,843 @@
   <sheetData>
     <row r="1" spans="1:7" ht="18">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>152</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>154</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>156</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>157</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="18">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="18">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="18">
       <c r="A5" s="4" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="18">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18">
       <c r="A7" s="4" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>31</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>49</v>
+        <v>236</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18">
       <c r="A8" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="7"/>
       <c r="E8" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="18">
       <c r="A9" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18">
       <c r="A10" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18">
       <c r="A12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>73</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18">
       <c r="A13" s="2" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="18">
       <c r="A14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18">
       <c r="A15" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18">
       <c r="A16" s="4" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F16" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>127</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="18">
       <c r="A17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B17" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>110</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18">
       <c r="A18" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G18" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>96</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18">
       <c r="A20" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>97</v>
-      </c>
       <c r="D20" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="F22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>131</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18">
       <c r="A23" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="G25" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18">
+      <c r="A26" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18">
+      <c r="A27" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18">
+      <c r="A28" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18">
+      <c r="A29" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18">
+      <c r="A30" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18">
+      <c r="A31" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="18">
+      <c r="A32" s="3" t="s">
         <v>159</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18">
+      <c r="A33" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="18">
+      <c r="A34" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18">
+      <c r="A35" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="18">
+      <c r="A36" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18">
+      <c r="A37" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Full and partial matching routine
</commit_message>
<xml_diff>
--- a/langame.xlsx
+++ b/langame.xlsx
@@ -1331,8 +1331,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1380,7 +1388,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1399,6 +1407,10 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1417,6 +1429,10 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1748,8 +1764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3029,10 +3045,10 @@
         <v>370</v>
       </c>
       <c r="D56" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>388</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>395</v>
@@ -3052,10 +3068,10 @@
         <v>368</v>
       </c>
       <c r="D57" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>389</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>382</v>
       </c>
       <c r="F57" s="2" t="s">
         <v>401</v>
@@ -3075,10 +3091,10 @@
         <v>367</v>
       </c>
       <c r="D58" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>393</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>383</v>
       </c>
       <c r="F58" s="2" t="s">
         <v>400</v>
@@ -3098,10 +3114,10 @@
         <v>369</v>
       </c>
       <c r="D59" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>384</v>
       </c>
       <c r="F59" s="2" t="s">
         <v>396</v>
@@ -3121,10 +3137,10 @@
         <v>371</v>
       </c>
       <c r="D60" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>391</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>385</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>399</v>
@@ -3144,10 +3160,10 @@
         <v>372</v>
       </c>
       <c r="D61" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>394</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>398</v>
@@ -3167,10 +3183,10 @@
         <v>373</v>
       </c>
       <c r="D62" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>387</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>397</v>

</xml_diff>

<commit_message>
Documented and License Added
</commit_message>
<xml_diff>
--- a/langame.xlsx
+++ b/langame.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="477">
   <si>
     <t>Hombre</t>
   </si>
@@ -1225,6 +1225,231 @@
   </si>
   <si>
     <t>Вторник</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>Mayo</t>
+  </si>
+  <si>
+    <t>Junio</t>
+  </si>
+  <si>
+    <t>Julio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Septiembre</t>
+  </si>
+  <si>
+    <t>Octubre</t>
+  </si>
+  <si>
+    <t>Noviembre</t>
+  </si>
+  <si>
+    <t>Diciembre</t>
+  </si>
+  <si>
+    <t>Janeiro</t>
+  </si>
+  <si>
+    <t>Fevereiro</t>
+  </si>
+  <si>
+    <t>Março</t>
+  </si>
+  <si>
+    <t>Maio</t>
+  </si>
+  <si>
+    <t>Junho</t>
+  </si>
+  <si>
+    <t>Julho</t>
+  </si>
+  <si>
+    <t>Setembro</t>
+  </si>
+  <si>
+    <t>Outubro</t>
+  </si>
+  <si>
+    <t>Novembro</t>
+  </si>
+  <si>
+    <t>Dezembro</t>
+  </si>
+  <si>
+    <t>Gennaio</t>
+  </si>
+  <si>
+    <t>Febbraio</t>
+  </si>
+  <si>
+    <t>Aprile</t>
+  </si>
+  <si>
+    <t>Maggio</t>
+  </si>
+  <si>
+    <t>Giugno</t>
+  </si>
+  <si>
+    <t>Iuglio</t>
+  </si>
+  <si>
+    <t>Settembre</t>
+  </si>
+  <si>
+    <t>Ottobre</t>
+  </si>
+  <si>
+    <t>Novembre</t>
+  </si>
+  <si>
+    <t>Dicembre</t>
+  </si>
+  <si>
+    <t>Gener</t>
+  </si>
+  <si>
+    <t>Febrer</t>
+  </si>
+  <si>
+    <t>Març</t>
+  </si>
+  <si>
+    <t>Maig</t>
+  </si>
+  <si>
+    <t>Juny</t>
+  </si>
+  <si>
+    <t>Juliol</t>
+  </si>
+  <si>
+    <t>Agost</t>
+  </si>
+  <si>
+    <t>Setembre</t>
+  </si>
+  <si>
+    <t>Desembre</t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>December</t>
+  </si>
+  <si>
+    <t>Janvier</t>
+  </si>
+  <si>
+    <t>Février</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Avril</t>
+  </si>
+  <si>
+    <t>Mai</t>
+  </si>
+  <si>
+    <t>Juin</t>
+  </si>
+  <si>
+    <t>Juillet</t>
+  </si>
+  <si>
+    <t>Août</t>
+  </si>
+  <si>
+    <t>Septembre</t>
+  </si>
+  <si>
+    <t>Décembre</t>
+  </si>
+  <si>
+    <t>Март</t>
+  </si>
+  <si>
+    <t>Апрель</t>
+  </si>
+  <si>
+    <t>Май</t>
+  </si>
+  <si>
+    <t>Январь</t>
+  </si>
+  <si>
+    <t>Февраль</t>
+  </si>
+  <si>
+    <t>Июнь</t>
+  </si>
+  <si>
+    <t>Июль</t>
+  </si>
+  <si>
+    <t>Август</t>
+  </si>
+  <si>
+    <t>Сентябрь</t>
+  </si>
+  <si>
+    <t>Октябрь</t>
+  </si>
+  <si>
+    <t>Ноябрь</t>
+  </si>
+  <si>
+    <t>Декабрь</t>
   </si>
 </sst>
 </file>
@@ -1762,10 +1987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3195,6 +3420,282 @@
         <v>380</v>
       </c>
     </row>
+    <row r="63" spans="1:7" ht="18">
+      <c r="A63" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="18">
+      <c r="A64" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>425</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>435</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>456</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18">
+      <c r="A65" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>457</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18">
+      <c r="A66" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18">
+      <c r="A67" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18">
+      <c r="A68" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>418</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18">
+      <c r="A69" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18">
+      <c r="A70" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>472</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18">
+      <c r="A71" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>420</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18">
+      <c r="A72" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18">
+      <c r="A73" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="18">
+      <c r="A74" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>423</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E74" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>454</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Accept repeated letters as partial matches
</commit_message>
<xml_diff>
--- a/langame.xlsx
+++ b/langame.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-35100" yWindow="-3460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="1140" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Words" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="833">
   <si>
     <t>Hombre</t>
   </si>
@@ -591,12 +591,6 @@
     <t>Abaix</t>
   </si>
   <si>
-    <t>Endavant</t>
-  </si>
-  <si>
-    <t>Darrera</t>
-  </si>
-  <si>
     <t>Dietro</t>
   </si>
   <si>
@@ -876,12 +870,6 @@
     <t>Por favor</t>
   </si>
   <si>
-    <t>Perdón</t>
-  </si>
-  <si>
-    <t>Disculpe</t>
-  </si>
-  <si>
     <t>De nada</t>
   </si>
   <si>
@@ -1783,6 +1771,753 @@
   </si>
   <si>
     <t>Hereusement!</t>
+  </si>
+  <si>
+    <t>Cocinar</t>
+  </si>
+  <si>
+    <t>Cucinare</t>
+  </si>
+  <si>
+    <t>Cozinhar</t>
+  </si>
+  <si>
+    <t>Cuinar</t>
+  </si>
+  <si>
+    <t>Cuisiner</t>
+  </si>
+  <si>
+    <t>Готовить</t>
+  </si>
+  <si>
+    <t>Cook</t>
+  </si>
+  <si>
+    <t>Говорить</t>
+  </si>
+  <si>
+    <t>Speak</t>
+  </si>
+  <si>
+    <t>Hablar</t>
+  </si>
+  <si>
+    <t>Falar</t>
+  </si>
+  <si>
+    <t>Parlare</t>
+  </si>
+  <si>
+    <t>Parlar</t>
+  </si>
+  <si>
+    <t>Parler</t>
+  </si>
+  <si>
+    <t>Trabajar</t>
+  </si>
+  <si>
+    <t>Trabalhar</t>
+  </si>
+  <si>
+    <t>Treballar</t>
+  </si>
+  <si>
+    <t>Работать</t>
+  </si>
+  <si>
+    <t>Work</t>
+  </si>
+  <si>
+    <t>Travailler</t>
+  </si>
+  <si>
+    <t>Lavorare</t>
+  </si>
+  <si>
+    <t>Ir</t>
+  </si>
+  <si>
+    <t>Andare</t>
+  </si>
+  <si>
+    <t>Venir</t>
+  </si>
+  <si>
+    <t>Vir</t>
+  </si>
+  <si>
+    <t>Anar</t>
+  </si>
+  <si>
+    <t>Aller</t>
+  </si>
+  <si>
+    <t>Идти</t>
+  </si>
+  <si>
+    <t>Go</t>
+  </si>
+  <si>
+    <t>Прийти</t>
+  </si>
+  <si>
+    <t>Come</t>
+  </si>
+  <si>
+    <t>Venire</t>
+  </si>
+  <si>
+    <t>Ser</t>
+  </si>
+  <si>
+    <t>Essere</t>
+  </si>
+  <si>
+    <t>Être</t>
+  </si>
+  <si>
+    <t>Be</t>
+  </si>
+  <si>
+    <t>Es</t>
+  </si>
+  <si>
+    <t>É</t>
+  </si>
+  <si>
+    <t>È</t>
+  </si>
+  <si>
+    <t>És</t>
+  </si>
+  <si>
+    <t>Est</t>
+  </si>
+  <si>
+    <t>Is</t>
+  </si>
+  <si>
+    <t>Leer</t>
+  </si>
+  <si>
+    <t>Leggere</t>
+  </si>
+  <si>
+    <t>Read</t>
+  </si>
+  <si>
+    <t>Ler</t>
+  </si>
+  <si>
+    <t>Llegir</t>
+  </si>
+  <si>
+    <t>Lire</t>
+  </si>
+  <si>
+    <t>Читать</t>
+  </si>
+  <si>
+    <t>Escribir</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>Écrire</t>
+  </si>
+  <si>
+    <t>Escriure</t>
+  </si>
+  <si>
+    <t>Scrivere</t>
+  </si>
+  <si>
+    <t>Escrever</t>
+  </si>
+  <si>
+    <t>Писать</t>
+  </si>
+  <si>
+    <t>Pequeño</t>
+  </si>
+  <si>
+    <t>Grande</t>
+  </si>
+  <si>
+    <t>Piccolo</t>
+  </si>
+  <si>
+    <t>Pequeno</t>
+  </si>
+  <si>
+    <t>Petit</t>
+  </si>
+  <si>
+    <t>Маленький</t>
+  </si>
+  <si>
+    <t>Большой</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Gran</t>
+  </si>
+  <si>
+    <t>Grand</t>
+  </si>
+  <si>
+    <t>Corto</t>
+  </si>
+  <si>
+    <t>Largo</t>
+  </si>
+  <si>
+    <t>Короткий</t>
+  </si>
+  <si>
+    <t>Curto</t>
+  </si>
+  <si>
+    <t>Lungo</t>
+  </si>
+  <si>
+    <t>Curt</t>
+  </si>
+  <si>
+    <t>Court</t>
+  </si>
+  <si>
+    <t>Long</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Llarg</t>
+  </si>
+  <si>
+    <t>Feo</t>
+  </si>
+  <si>
+    <t>Lleig</t>
+  </si>
+  <si>
+    <t>Bonito, Lindo</t>
+  </si>
+  <si>
+    <t>Bonic, Maco</t>
+  </si>
+  <si>
+    <t>Beau, Jolie</t>
+  </si>
+  <si>
+    <t>Bello, Carino</t>
+  </si>
+  <si>
+    <t>Beautiful, Pretty</t>
+  </si>
+  <si>
+    <t>Красивий</t>
+  </si>
+  <si>
+    <t>Гладкий</t>
+  </si>
+  <si>
+    <t>Ugly</t>
+  </si>
+  <si>
+    <t>Длинный</t>
+  </si>
+  <si>
+    <t>Know</t>
+  </si>
+  <si>
+    <t>Знать</t>
+  </si>
+  <si>
+    <t>Saber, Conocer</t>
+  </si>
+  <si>
+    <t>Saber, Conhecer</t>
+  </si>
+  <si>
+    <t>Sapere, Conoscere</t>
+  </si>
+  <si>
+    <t>Sapiguer, Conèixer</t>
+  </si>
+  <si>
+    <t>Savoir, Connaître</t>
+  </si>
+  <si>
+    <t>Pensar</t>
+  </si>
+  <si>
+    <t>Think</t>
+  </si>
+  <si>
+    <t>Pensare</t>
+  </si>
+  <si>
+    <t>Penser</t>
+  </si>
+  <si>
+    <t>Думать</t>
+  </si>
+  <si>
+    <t>Aprender</t>
+  </si>
+  <si>
+    <t>Recordar</t>
+  </si>
+  <si>
+    <t>Olvidar</t>
+  </si>
+  <si>
+    <t>Creer</t>
+  </si>
+  <si>
+    <t>Believe</t>
+  </si>
+  <si>
+    <t>Acreditar</t>
+  </si>
+  <si>
+    <t>Credere</t>
+  </si>
+  <si>
+    <t>Creure</t>
+  </si>
+  <si>
+    <t>Croir</t>
+  </si>
+  <si>
+    <t>Oblidar</t>
+  </si>
+  <si>
+    <t>Oublier</t>
+  </si>
+  <si>
+    <t>Forget</t>
+  </si>
+  <si>
+    <t>Remember</t>
+  </si>
+  <si>
+    <t>Learn</t>
+  </si>
+  <si>
+    <t>Imparare</t>
+  </si>
+  <si>
+    <t>Учить</t>
+  </si>
+  <si>
+    <t>Aprendre</t>
+  </si>
+  <si>
+    <t>Lembrar</t>
+  </si>
+  <si>
+    <t>Apprendre</t>
+  </si>
+  <si>
+    <t>Souvenir</t>
+  </si>
+  <si>
+    <t>Ricordare</t>
+  </si>
+  <si>
+    <t>Querer</t>
+  </si>
+  <si>
+    <t>Vogliere</t>
+  </si>
+  <si>
+    <t>Voler</t>
+  </si>
+  <si>
+    <t>Vouloir</t>
+  </si>
+  <si>
+    <t>Хотеть</t>
+  </si>
+  <si>
+    <t>Want</t>
+  </si>
+  <si>
+    <t>Poder</t>
+  </si>
+  <si>
+    <t>Can</t>
+  </si>
+  <si>
+    <t>Potere</t>
+  </si>
+  <si>
+    <t>Poguer</t>
+  </si>
+  <si>
+    <t>Povoir</t>
+  </si>
+  <si>
+    <t>Уметь, Мочь</t>
+  </si>
+  <si>
+    <t>VERBOS</t>
+  </si>
+  <si>
+    <t>Recordar, Enrecordar</t>
+  </si>
+  <si>
+    <t>Помнить</t>
+  </si>
+  <si>
+    <t>Понимать</t>
+  </si>
+  <si>
+    <t>Забывать</t>
+  </si>
+  <si>
+    <t>Верить</t>
+  </si>
+  <si>
+    <t>Esquecer</t>
+  </si>
+  <si>
+    <t>Dimenticare</t>
+  </si>
+  <si>
+    <t>Capire</t>
+  </si>
+  <si>
+    <t>Entender, Comprender</t>
+  </si>
+  <si>
+    <t>Comprendre</t>
+  </si>
+  <si>
+    <t>Entendre</t>
+  </si>
+  <si>
+    <t>Understand</t>
+  </si>
+  <si>
+    <t>Listen</t>
+  </si>
+  <si>
+    <t>Hear</t>
+  </si>
+  <si>
+    <t>Escoltar</t>
+  </si>
+  <si>
+    <t>Escuchar</t>
+  </si>
+  <si>
+    <t>Écouter</t>
+  </si>
+  <si>
+    <t>Ascoltare</t>
+  </si>
+  <si>
+    <t>Escutar</t>
+  </si>
+  <si>
+    <t>Ouvir</t>
+  </si>
+  <si>
+    <t>Oír</t>
+  </si>
+  <si>
+    <t>Слушать</t>
+  </si>
+  <si>
+    <t>Слышать</t>
+  </si>
+  <si>
+    <t>Sentire</t>
+  </si>
+  <si>
+    <t>Sento</t>
+  </si>
+  <si>
+    <t>Mirar</t>
+  </si>
+  <si>
+    <t>Ver</t>
+  </si>
+  <si>
+    <t>See</t>
+  </si>
+  <si>
+    <t>Look, Watch</t>
+  </si>
+  <si>
+    <t>Смотреть</t>
+  </si>
+  <si>
+    <t>Olhar</t>
+  </si>
+  <si>
+    <t>Guardare</t>
+  </si>
+  <si>
+    <t>Veure</t>
+  </si>
+  <si>
+    <t>Regarder</t>
+  </si>
+  <si>
+    <t>Voir</t>
+  </si>
+  <si>
+    <t>Search</t>
+  </si>
+  <si>
+    <t>Find</t>
+  </si>
+  <si>
+    <t>Vedere</t>
+  </si>
+  <si>
+    <t>Cercare, Ricercare</t>
+  </si>
+  <si>
+    <t>Buscar</t>
+  </si>
+  <si>
+    <t>Procurar</t>
+  </si>
+  <si>
+    <t>Buscar, Cercar</t>
+  </si>
+  <si>
+    <t>Chercher, Rechercher</t>
+  </si>
+  <si>
+    <t>Искать</t>
+  </si>
+  <si>
+    <t>Находить</t>
+  </si>
+  <si>
+    <t>Encontrar</t>
+  </si>
+  <si>
+    <t>Pensar, Achar</t>
+  </si>
+  <si>
+    <t>Encontrar, Achar</t>
+  </si>
+  <si>
+    <t>Trovare</t>
+  </si>
+  <si>
+    <t>Trobar</t>
+  </si>
+  <si>
+    <t>Trouver</t>
+  </si>
+  <si>
+    <t>Видеть</t>
+  </si>
+  <si>
+    <t>Olfatear</t>
+  </si>
+  <si>
+    <t>Oler</t>
+  </si>
+  <si>
+    <t>Sentir</t>
+  </si>
+  <si>
+    <t>Smell</t>
+  </si>
+  <si>
+    <t>Sniff</t>
+  </si>
+  <si>
+    <t>Renifler</t>
+  </si>
+  <si>
+    <t>Olorar</t>
+  </si>
+  <si>
+    <t>Ensumar</t>
+  </si>
+  <si>
+    <t>Farejar</t>
+  </si>
+  <si>
+    <t>Cheirar</t>
+  </si>
+  <si>
+    <t>Annusare</t>
+  </si>
+  <si>
+    <t>Нюхать</t>
+  </si>
+  <si>
+    <t>Нахнуть</t>
+  </si>
+  <si>
+    <t>Odorare</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Bad</t>
+  </si>
+  <si>
+    <t>Хороший</t>
+  </si>
+  <si>
+    <t>Плохой</t>
+  </si>
+  <si>
+    <t>ADJETIVOS</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Люди</t>
+  </si>
+  <si>
+    <t>Gente</t>
+  </si>
+  <si>
+    <t>Gens</t>
+  </si>
+  <si>
+    <t>Gent</t>
+  </si>
+  <si>
+    <t>Comer</t>
+  </si>
+  <si>
+    <t>Beber</t>
+  </si>
+  <si>
+    <t>Eat</t>
+  </si>
+  <si>
+    <t>Drink</t>
+  </si>
+  <si>
+    <t>Есть</t>
+  </si>
+  <si>
+    <t>Пить</t>
+  </si>
+  <si>
+    <t>Mangiare</t>
+  </si>
+  <si>
+    <t>Bere</t>
+  </si>
+  <si>
+    <t>Beure</t>
+  </si>
+  <si>
+    <t>Menjar</t>
+  </si>
+  <si>
+    <t>Manger</t>
+  </si>
+  <si>
+    <t>Boire</t>
+  </si>
+  <si>
+    <t>EXPRESIONES</t>
+  </si>
+  <si>
+    <t>Bueno</t>
+  </si>
+  <si>
+    <t>Malo</t>
+  </si>
+  <si>
+    <t>Buono</t>
+  </si>
+  <si>
+    <t>Bon</t>
+  </si>
+  <si>
+    <t>Bom</t>
+  </si>
+  <si>
+    <t>Bo</t>
+  </si>
+  <si>
+    <t>Dolent</t>
+  </si>
+  <si>
+    <t>Ruim, Mau</t>
+  </si>
+  <si>
+    <t>Mauvais</t>
+  </si>
+  <si>
+    <t>Feio</t>
+  </si>
+  <si>
+    <t>Brutto</t>
+  </si>
+  <si>
+    <t>Cattivo</t>
+  </si>
+  <si>
+    <t>Perdón (Atención)</t>
+  </si>
+  <si>
+    <t>Perdón (Disculpa)</t>
+  </si>
+  <si>
+    <t>Endarrera, Darrera</t>
+  </si>
+  <si>
+    <t>Endavant, Davant</t>
+  </si>
+  <si>
+    <t>Siempre</t>
+  </si>
+  <si>
+    <t>Nunca</t>
+  </si>
+  <si>
+    <t>Всегда</t>
+  </si>
+  <si>
+    <t>Никогда</t>
+  </si>
+  <si>
+    <t>Never</t>
+  </si>
+  <si>
+    <t>Always</t>
+  </si>
+  <si>
+    <t>Sempre</t>
+  </si>
+  <si>
+    <t>Toujours</t>
+  </si>
+  <si>
+    <t>Jamais</t>
+  </si>
+  <si>
+    <t>Nunca, Jamás</t>
   </si>
 </sst>
 </file>
@@ -1883,8 +2618,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1945,9 +2698,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1973,6 +2726,15 @@
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1998,6 +2760,15 @@
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2327,10 +3098,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G92"/>
+  <dimension ref="A1:G133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E94" sqref="E94"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2338,7 +3109,7 @@
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" customWidth="1"/>
     <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.5" bestFit="1" customWidth="1"/>
@@ -2461,22 +3232,22 @@
     </row>
     <row r="6" spans="1:7" ht="18">
       <c r="A6" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>30</v>
@@ -2756,733 +3527,733 @@
     </row>
     <row r="19" spans="1:7" ht="18">
       <c r="A19" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>462</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>462</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>466</v>
-      </c>
       <c r="D19" s="6" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>461</v>
+      </c>
+      <c r="G19" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18">
       <c r="A20" s="5" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18">
       <c r="A21" s="6" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>471</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>472</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>490</v>
+      </c>
+      <c r="G21" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>478</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>494</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="18">
       <c r="A22" s="5" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18">
       <c r="A23" s="5" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18">
       <c r="A24" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>496</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="G24" s="2" t="s">
         <v>497</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>501</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18">
       <c r="A25" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18">
       <c r="A26" s="5" t="s">
-        <v>107</v>
+        <v>791</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>107</v>
+        <v>791</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>107</v>
+        <v>791</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>107</v>
+        <v>793</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>111</v>
+        <v>792</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>790</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>112</v>
+        <v>789</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18">
       <c r="A27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18">
+      <c r="A28" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B28" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18">
-      <c r="A28" s="6" t="s">
+    <row r="29" spans="1:7" ht="18">
+      <c r="A29" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D29" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E29" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="F29" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="G28" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="18">
-      <c r="A29" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18">
       <c r="A30" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18">
+      <c r="A31" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B31" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D31" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="E30" s="6" t="s">
+      <c r="E31" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="F30" s="6" t="s">
+      <c r="F31" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18">
-      <c r="A31" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="18">
       <c r="A32" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18">
       <c r="A33" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="18">
       <c r="A34" s="2" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="F34" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>173</v>
+      </c>
       <c r="G34" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="18">
       <c r="A35" s="2" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>206</v>
-      </c>
+        <v>168</v>
+      </c>
+      <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="18">
       <c r="A36" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>534</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>535</v>
-      </c>
       <c r="F36" s="2" t="s">
-        <v>536</v>
+        <v>204</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>537</v>
+        <v>205</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="18">
       <c r="A37" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>174</v>
+        <v>199</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>533</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="18">
       <c r="A38" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="18">
       <c r="A39" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="18">
       <c r="A40" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18">
       <c r="A41" s="2" t="s">
-        <v>179</v>
+        <v>147</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>214</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="18">
       <c r="A42" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>149</v>
+        <v>212</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>191</v>
+        <v>822</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="18">
       <c r="A43" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>281</v>
+        <v>180</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>821</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="18">
       <c r="A44" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>225</v>
+        <v>256</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="18">
       <c r="A45" s="2" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>231</v>
+        <v>239</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>237</v>
+        <v>270</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>236</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="18">
       <c r="A46" s="2" t="s">
-        <v>227</v>
+        <v>233</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="18">
       <c r="A47" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>240</v>
+        <v>225</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="18">
       <c r="A48" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="18">
       <c r="A49" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>244</v>
+        <v>227</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>253</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="18">
       <c r="A50" s="2" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>265</v>
@@ -3490,232 +4261,232 @@
     </row>
     <row r="51" spans="1:7" ht="18">
       <c r="A51" s="2" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>251</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>278</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="18">
       <c r="A52" s="2" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>288</v>
+        <v>248</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>290</v>
+        <v>249</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>297</v>
+        <v>261</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>291</v>
+        <v>268</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>294</v>
+        <v>264</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="18">
       <c r="A53" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="C53" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>289</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>300</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="18">
       <c r="A54" s="2" t="s">
-        <v>284</v>
+        <v>820</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="18">
       <c r="A55" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="18">
       <c r="A56" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>287</v>
+        <v>303</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="18">
       <c r="A57" s="2" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>316</v>
+        <v>283</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>315</v>
+        <v>298</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="18">
       <c r="A58" s="2" t="s">
-        <v>221</v>
+        <v>310</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>338</v>
+        <v>315</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>333</v>
+        <v>316</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="18">
       <c r="A59" s="2" t="s">
-        <v>222</v>
+        <v>823</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>322</v>
+        <v>829</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>325</v>
+        <v>829</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>328</v>
+        <v>829</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>331</v>
+        <v>830</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>336</v>
+        <v>825</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>334</v>
+        <v>828</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="18">
       <c r="A60" s="2" t="s">
-        <v>223</v>
+        <v>832</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>323</v>
+        <v>824</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>326</v>
+        <v>437</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>329</v>
+        <v>437</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>332</v>
+        <v>831</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>337</v>
+        <v>826</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>335</v>
+        <v>827</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="18">
@@ -3723,22 +4494,22 @@
         <v>219</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>344</v>
+        <v>317</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>363</v>
+        <v>323</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>377</v>
+        <v>334</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>356</v>
+        <v>329</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="18">
@@ -3746,689 +4517,1615 @@
         <v>220</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>345</v>
+        <v>318</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>350</v>
+        <v>321</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>364</v>
+        <v>324</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>371</v>
+        <v>327</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>383</v>
+        <v>332</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>357</v>
+        <v>330</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="18">
       <c r="A63" s="2" t="s">
-        <v>339</v>
+        <v>221</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>346</v>
+        <v>319</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>349</v>
+        <v>322</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>365</v>
+        <v>325</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>375</v>
+        <v>328</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>382</v>
+        <v>333</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>358</v>
+        <v>331</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="18">
       <c r="A64" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>347</v>
-      </c>
       <c r="C64" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D64" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E64" s="2" t="s">
-        <v>374</v>
-      </c>
       <c r="F64" s="2" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="18">
       <c r="A65" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>348</v>
-      </c>
       <c r="C65" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>379</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="18">
       <c r="A66" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C66" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="G66" s="2" t="s">
         <v>354</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="18">
       <c r="A67" s="2" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>343</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F67" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="18">
       <c r="A68" s="2" t="s">
-        <v>384</v>
+        <v>337</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>406</v>
+        <v>349</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>437</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>450</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>425</v>
+        <v>363</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="18">
       <c r="A69" s="2" t="s">
-        <v>385</v>
+        <v>338</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>397</v>
+        <v>338</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>407</v>
+        <v>350</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>426</v>
+        <v>364</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="18">
       <c r="A70" s="2" t="s">
-        <v>386</v>
+        <v>339</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>398</v>
+        <v>339</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>386</v>
+        <v>351</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="F70" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>427</v>
+        <v>365</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>375</v>
+      </c>
+      <c r="G70" s="2" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="18">
       <c r="A71" s="2" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>387</v>
+        <v>412</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="18">
       <c r="A72" s="2" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="18">
       <c r="A73" s="2" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>410</v>
+        <v>382</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="18">
       <c r="A74" s="2" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>401</v>
+        <v>383</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>421</v>
+        <v>383</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="18">
       <c r="A75" s="2" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>391</v>
+        <v>405</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="18">
       <c r="A76" s="2" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="18">
       <c r="A77" s="2" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>393</v>
+        <v>417</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>393</v>
+        <v>439</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="18">
       <c r="A78" s="2" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>404</v>
+        <v>387</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>414</v>
+        <v>387</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>414</v>
+        <v>440</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="18">
       <c r="A79" s="2" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="18">
       <c r="A80" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>563</v>
+        <v>389</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>399</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>514</v>
+        <v>409</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>389</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>545</v>
+        <v>389</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>571</v>
-      </c>
-      <c r="G80" s="4" t="s">
-        <v>508</v>
+        <v>452</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="18">
       <c r="A81" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>564</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>543</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>562</v>
+        <v>390</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>546</v>
+        <v>410</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>572</v>
-      </c>
-      <c r="G81" s="4" t="s">
-        <v>509</v>
+        <v>453</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="18">
       <c r="A82" s="2" t="s">
-        <v>523</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>524</v>
+        <v>391</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>401</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>524</v>
+        <v>411</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>522</v>
+        <v>420</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>442</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>574</v>
-      </c>
-      <c r="G82" s="4" t="s">
-        <v>521</v>
+        <v>454</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="18">
       <c r="A83" s="2" t="s">
-        <v>516</v>
+        <v>510</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>560</v>
+        <v>510</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="18">
       <c r="A84" s="2" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>517</v>
+        <v>560</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="18">
       <c r="A85" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>566</v>
-      </c>
-      <c r="C85" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>557</v>
-      </c>
-      <c r="E85" s="3" t="s">
-        <v>550</v>
-      </c>
       <c r="F85" s="3" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="G85" s="4" t="s">
-        <v>511</v>
+        <v>517</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="18">
       <c r="A86" s="2" t="s">
-        <v>519</v>
+        <v>512</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="C86" s="3" t="s">
-        <v>528</v>
+        <v>561</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>516</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="G86" s="4" t="s">
-        <v>512</v>
+        <v>506</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="18">
       <c r="A87" s="2" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>530</v>
+        <v>513</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>530</v>
+        <v>540</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>579</v>
-      </c>
-      <c r="G87" s="7" t="s">
-        <v>538</v>
+        <v>569</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="18">
       <c r="A88" s="2" t="s">
-        <v>531</v>
+        <v>514</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>532</v>
+        <v>553</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="F88" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="18">
+      <c r="A89" s="2" t="s">
+        <v>515</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="18">
+      <c r="A90" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="18">
+      <c r="A91" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="18">
+      <c r="A92" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="B92" s="5" t="s">
+        <v>564</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>552</v>
+      </c>
+      <c r="E92" s="5" t="s">
+        <v>548</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>576</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="18">
+      <c r="A93" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="B93" s="5" t="s">
+        <v>566</v>
+      </c>
+      <c r="C93" s="5" t="s">
+        <v>537</v>
+      </c>
+      <c r="D93" s="5" t="s">
+        <v>551</v>
+      </c>
+      <c r="E93" s="5" t="s">
+        <v>549</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>577</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="18">
+      <c r="A94" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+      <c r="D94" s="2"/>
+      <c r="E94" s="2"/>
+      <c r="F94" s="2"/>
+      <c r="G94" s="2"/>
+    </row>
+    <row r="95" spans="1:7" ht="18">
+      <c r="A95" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="D95" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="F95" s="2"/>
+      <c r="G95" s="2" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="18">
+      <c r="A96" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="D96" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="E96" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="F96" s="2"/>
+      <c r="G96" s="2" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="18">
+      <c r="A97" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>706</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="G97" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="18">
+      <c r="A98" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>713</v>
+      </c>
+      <c r="D98" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>715</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>716</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="18">
+      <c r="A99" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>605</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>606</v>
+      </c>
+      <c r="D99" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="18">
+      <c r="A100" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>607</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="18">
+      <c r="A101" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>627</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>631</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="18">
+      <c r="A102" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="D102" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>635</v>
+      </c>
+      <c r="F102" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="G102" s="2" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="18">
+      <c r="A103" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="D103" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>774</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="18">
+      <c r="A104" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="D104" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="E104" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="G104" s="2" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="18">
+      <c r="A105" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>748</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>749</v>
+      </c>
+      <c r="D105" s="2" t="s">
+        <v>743</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>751</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="G105" s="2" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="18">
+      <c r="A106" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>750</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="18">
+      <c r="A107" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="D107" s="2" t="s">
+        <v>759</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>760</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>761</v>
+      </c>
+      <c r="G107" s="2" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="18">
+      <c r="A108" s="2" t="s">
+        <v>763</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>765</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="D108" s="2" t="s">
+        <v>767</v>
+      </c>
+      <c r="E108" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="G108" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="18">
+      <c r="A109" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="D109" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="E109" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>739</v>
+      </c>
+      <c r="G109" s="2" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="18">
+      <c r="A110" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>737</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>742</v>
+      </c>
+      <c r="E110" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="F110" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="18">
+      <c r="A111" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="G111" s="2" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="18">
+      <c r="A112" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>725</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>727</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>720</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="18">
+      <c r="A113" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="E113" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="G113" s="2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="18">
+      <c r="A114" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="E114" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>719</v>
+      </c>
+      <c r="G114" s="2" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="18">
+      <c r="A115" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>723</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>724</v>
+      </c>
+      <c r="D115" s="2" t="s">
+        <v>693</v>
+      </c>
+      <c r="E115" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>721</v>
+      </c>
+      <c r="G115" s="2" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="18">
+      <c r="A116" s="2" t="s">
+        <v>674</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>675</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="D116" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="E116" s="2" t="s">
+        <v>678</v>
+      </c>
+      <c r="F116" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="18">
+      <c r="A117" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>764</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>679</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>683</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="18">
+      <c r="A118" s="2" t="s">
+        <v>687</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>689</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D118" s="2" t="s">
+        <v>691</v>
+      </c>
+      <c r="E118" s="2" t="s">
+        <v>692</v>
+      </c>
+      <c r="F118" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="18">
+      <c r="A119" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="D119" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="F119" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="18">
+      <c r="A120" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="G120" s="2" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="18">
+      <c r="A121" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="B121" s="3" t="s">
+        <v>794</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>803</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>804</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G121" s="2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="18">
+      <c r="A122" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>795</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>801</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>802</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>805</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>799</v>
+      </c>
+      <c r="G122" s="2" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="18">
+      <c r="A123" s="2" t="s">
+        <v>788</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
+      <c r="E123" s="2"/>
+      <c r="F123" s="2"/>
+      <c r="G123" s="2"/>
+    </row>
+    <row r="124" spans="1:7" ht="18">
+      <c r="A124" s="2" t="s">
+        <v>807</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>811</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>809</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>810</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>786</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="18">
+      <c r="A125" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>814</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>818</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>813</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="G125" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="18">
+      <c r="A126" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="D126" s="2" t="s">
+        <v>664</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="F126" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="G126" s="2" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="18">
+      <c r="A127" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>816</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>817</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="F127" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="G127" s="2" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="18">
+      <c r="A128" s="2" t="s">
+        <v>640</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="F128" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="18">
+      <c r="A129" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="D129" s="2" t="s">
+        <v>649</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>650</v>
+      </c>
+      <c r="F129" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="G129" s="2" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="18">
+      <c r="A130" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="D130" s="2" t="s">
+        <v>656</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="F130" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="G130" s="2" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="18">
+      <c r="A131" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>658</v>
+      </c>
+      <c r="F131" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="G131" s="2" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="18">
+      <c r="A132" s="2" t="s">
+        <v>806</v>
+      </c>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+      <c r="F132" s="8"/>
+      <c r="G132" s="8"/>
+    </row>
+    <row r="133" spans="1:7" ht="18">
+      <c r="A133" s="3" t="s">
         <v>578</v>
       </c>
-      <c r="G88" s="7" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="18">
-      <c r="A89" s="5" t="s">
-        <v>569</v>
-      </c>
-      <c r="B89" s="5" t="s">
-        <v>568</v>
-      </c>
-      <c r="C89" s="5" t="s">
-        <v>542</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>556</v>
-      </c>
-      <c r="E89" s="5" t="s">
-        <v>552</v>
-      </c>
-      <c r="F89" s="6" t="s">
+      <c r="B133" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="D133" s="3" t="s">
         <v>580</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="18">
-      <c r="A90" s="5" t="s">
-        <v>540</v>
-      </c>
-      <c r="B90" s="5" t="s">
-        <v>570</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>541</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>555</v>
-      </c>
-      <c r="E90" s="5" t="s">
-        <v>553</v>
-      </c>
-      <c r="F90" s="6" t="s">
+      <c r="E133" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="F133" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="G133" s="3" t="s">
         <v>581</v>
-      </c>
-      <c r="G90" s="3" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="18">
-      <c r="A92" s="8" t="s">
-        <v>582</v>
-      </c>
-      <c r="B92" s="8" t="s">
-        <v>582</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>583</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>584</v>
-      </c>
-      <c r="E92" s="8" t="s">
-        <v>587</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>586</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>